<commit_message>
fix metadata files add rsv bioproject and change IL0005 name to be different from MPOX and change sex to host_sex, age to host_age
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/rsv_test_metadata.xlsx
+++ b/assets/sample_metadata/rsv_test_metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\sample_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19114AC-41DF-426F-9F89-AAB97EB22AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E99BA2-C56B-49FE-869A-A12F076A6241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="411">
   <si>
     <t>Strategy</t>
   </si>
@@ -1168,9 +1168,6 @@
     <t>test_field_3</t>
   </si>
   <si>
-    <t>IL0005</t>
-  </si>
-  <si>
     <t>IL</t>
   </si>
   <si>
@@ -1180,9 +1177,6 @@
     <t xml:space="preserve"> ivar 0.1; samtools 1.7; bwa 0.7.17;  SPAdes 3.13.0; CLC 23</t>
   </si>
   <si>
-    <t>MPXV_IL0005</t>
-  </si>
-  <si>
     <t>ncbi-spuid</t>
   </si>
   <si>
@@ -1231,9 +1225,6 @@
     <t>gff_path</t>
   </si>
   <si>
-    <t>RSV_USA_2022_IL0005</t>
-  </si>
-  <si>
     <t>John Smith; Jane Smith</t>
   </si>
   <si>
@@ -1259,6 +1250,27 @@
   </si>
   <si>
     <t>authors</t>
+  </si>
+  <si>
+    <t>host_sex</t>
+  </si>
+  <si>
+    <t>host_age</t>
+  </si>
+  <si>
+    <t>RSV_TEST</t>
+  </si>
+  <si>
+    <t>DRR152972</t>
+  </si>
+  <si>
+    <t>PRJDB7467TEST</t>
+  </si>
+  <si>
+    <t>RSV_USA_DRR152972</t>
+  </si>
+  <si>
+    <t>RSV_DRR152972</t>
   </si>
 </sst>
 </file>
@@ -1517,7 +1529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1668,6 +1680,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1976,8 +1994,8 @@
   </sheetPr>
   <dimension ref="A1:BB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2033,192 +2051,196 @@
     </row>
     <row r="2" spans="1:54" ht="18.75" customHeight="1">
       <c r="A2" s="45" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B2" s="45" t="s">
+        <v>379</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2" s="45" t="s">
         <v>381</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="E2" s="45" t="s">
+        <v>400</v>
+      </c>
+      <c r="F2" s="47" t="s">
         <v>382</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="G2" s="45" t="s">
+        <v>403</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>386</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>387</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>388</v>
+      </c>
+      <c r="K2" s="47" t="s">
+        <v>389</v>
+      </c>
+      <c r="L2" s="47" t="s">
+        <v>390</v>
+      </c>
+      <c r="M2" s="53" t="s">
+        <v>368</v>
+      </c>
+      <c r="N2" s="47" t="s">
+        <v>385</v>
+      </c>
+      <c r="O2" s="47"/>
+      <c r="P2" s="45" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q2" s="45" t="s">
+        <v>370</v>
+      </c>
+      <c r="R2" s="45" t="s">
+        <v>371</v>
+      </c>
+      <c r="S2" s="45" t="s">
+        <v>372</v>
+      </c>
+      <c r="T2" s="45" t="s">
+        <v>287</v>
+      </c>
+      <c r="U2" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="V2" s="45" t="s">
+        <v>324</v>
+      </c>
+      <c r="W2" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="X2" s="45" t="s">
+        <v>325</v>
+      </c>
+      <c r="Y2" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z2" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="AA2" s="45" t="s">
+        <v>405</v>
+      </c>
+      <c r="AB2" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC2" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD2" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="AE2" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF2" s="54" t="s">
+        <v>242</v>
+      </c>
+      <c r="AG2" s="48" t="s">
+        <v>391</v>
+      </c>
+      <c r="AH2" s="48" t="s">
+        <v>394</v>
+      </c>
+      <c r="AI2" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ2" s="53" t="s">
+        <v>288</v>
+      </c>
+      <c r="AK2" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="AL2" s="45" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM2" s="45" t="s">
+        <v>291</v>
+      </c>
+      <c r="AN2" s="45" t="s">
+        <v>292</v>
+      </c>
+      <c r="AO2" s="45" t="s">
+        <v>327</v>
+      </c>
+      <c r="AP2" s="45" t="s">
         <v>383</v>
-      </c>
-      <c r="E2" s="45" t="s">
-        <v>403</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>384</v>
-      </c>
-      <c r="G2" s="45" t="s">
-        <v>406</v>
-      </c>
-      <c r="H2" s="47" t="s">
-        <v>388</v>
-      </c>
-      <c r="I2" s="47" t="s">
-        <v>389</v>
-      </c>
-      <c r="J2" s="47" t="s">
-        <v>390</v>
-      </c>
-      <c r="K2" s="47" t="s">
-        <v>391</v>
-      </c>
-      <c r="L2" s="47" t="s">
-        <v>392</v>
-      </c>
-      <c r="M2" s="37" t="s">
-        <v>368</v>
-      </c>
-      <c r="N2" s="47" t="s">
-        <v>387</v>
-      </c>
-      <c r="O2" s="47" t="s">
-        <v>384</v>
-      </c>
-      <c r="P2" s="20" t="s">
-        <v>369</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>370</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>371</v>
-      </c>
-      <c r="S2" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="T2" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="U2" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="V2" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="W2" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="X2" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="Y2" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z2" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="AA2" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="AB2" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="AC2" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="AD2" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="AE2" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="AF2" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="AG2" s="48" t="s">
-        <v>393</v>
-      </c>
-      <c r="AH2" s="48" t="s">
-        <v>396</v>
-      </c>
-      <c r="AI2" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="AJ2" s="37" t="s">
-        <v>288</v>
-      </c>
-      <c r="AK2" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="AL2" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="AM2" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="AN2" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="AO2" s="20" t="s">
-        <v>327</v>
-      </c>
-      <c r="AP2" s="45" t="s">
-        <v>385</v>
       </c>
       <c r="AQ2" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AR2" s="20" t="s">
+      <c r="AR2" s="45" t="s">
         <v>299</v>
       </c>
-      <c r="AS2" s="37" t="s">
+      <c r="AS2" s="53" t="s">
         <v>293</v>
       </c>
-      <c r="AT2" s="20" t="s">
+      <c r="AT2" s="45" t="s">
         <v>328</v>
       </c>
-      <c r="AU2" s="20" t="s">
+      <c r="AU2" s="45" t="s">
         <v>295</v>
       </c>
-      <c r="AV2" s="20" t="s">
+      <c r="AV2" s="45" t="s">
         <v>296</v>
       </c>
-      <c r="AW2" s="20" t="s">
+      <c r="AW2" s="45" t="s">
         <v>297</v>
       </c>
-      <c r="AX2" s="20" t="s">
+      <c r="AX2" s="45" t="s">
         <v>329</v>
       </c>
-      <c r="AY2" s="20" t="s">
+      <c r="AY2" s="45" t="s">
         <v>300</v>
       </c>
-      <c r="AZ2" s="21" t="s">
+      <c r="AZ2" s="54" t="s">
         <v>373</v>
       </c>
-      <c r="BA2" s="21" t="s">
+      <c r="BA2" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="BB2" s="21" t="s">
+      <c r="BB2" s="54" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:54" ht="18.75" customHeight="1">
       <c r="A3" t="s">
-        <v>376</v>
+        <v>407</v>
       </c>
       <c r="B3" t="s">
-        <v>397</v>
+        <v>409</v>
+      </c>
+      <c r="C3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D3" t="s">
+        <v>408</v>
       </c>
       <c r="E3" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F3" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G3" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="M3" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
       <c r="Q3" t="s">
         <v>257</v>
       </c>
       <c r="R3" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="S3" t="s">
         <v>350</v>
@@ -2227,26 +2249,25 @@
         <v>307</v>
       </c>
       <c r="U3" t="s">
+        <v>376</v>
+      </c>
+      <c r="X3" t="s">
         <v>377</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" s="36"/>
+      <c r="AD3" s="36" t="s">
         <v>378</v>
-      </c>
-      <c r="Z3" s="36"/>
-      <c r="AD3" t="s">
-        <v>379</v>
       </c>
       <c r="AF3" s="14">
         <v>40</v>
       </c>
       <c r="AG3" s="49" t="s">
-        <v>400</v>
-      </c>
-      <c r="AH3" s="14"/>
-      <c r="AI3" t="s">
-        <v>380</v>
-      </c>
-      <c r="AJ3" t="s">
+        <v>397</v>
+      </c>
+      <c r="AI3" s="36" t="s">
+        <v>410</v>
+      </c>
+      <c r="AJ3" s="36" t="s">
         <v>216</v>
       </c>
       <c r="AK3" t="s">
@@ -2262,20 +2283,20 @@
         <v>310</v>
       </c>
       <c r="AP3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AQ3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="AR3" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="AS3" s="36"/>
       <c r="AZ3" s="14">
         <v>5</v>
       </c>
       <c r="BA3" s="50" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="BB3" s="14">
         <v>0</v>
@@ -2283,47 +2304,51 @@
     </row>
     <row r="4" spans="1:54" ht="18.75" customHeight="1">
       <c r="Z4" s="36"/>
+      <c r="AD4" s="36"/>
       <c r="AF4" s="14"/>
       <c r="AG4" s="14"/>
-      <c r="AH4" s="14"/>
+      <c r="AI4" s="36"/>
+      <c r="AJ4" s="36"/>
       <c r="AS4" s="36"/>
       <c r="AZ4" s="14"/>
       <c r="BA4" s="49"/>
       <c r="BB4" s="14"/>
     </row>
-    <row r="5" spans="1:54" ht="18.75" customHeight="1">
+    <row r="5" spans="1:54">
       <c r="Z5" s="36"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AS5" s="36"/>
-      <c r="AZ5" s="14"/>
-      <c r="BA5" s="50"/>
-      <c r="BB5" s="14"/>
+      <c r="AD5" s="36"/>
+      <c r="AI5" s="36"/>
+      <c r="AJ5" s="36"/>
     </row>
     <row r="6" spans="1:54" ht="18.75" customHeight="1">
       <c r="Z6" s="36"/>
+      <c r="AD6" s="36"/>
       <c r="AF6" s="14"/>
       <c r="AG6" s="14"/>
-      <c r="AH6" s="14"/>
+      <c r="AI6" s="36"/>
+      <c r="AJ6" s="36"/>
       <c r="AS6" s="36"/>
       <c r="BA6" s="50"/>
       <c r="BB6" s="14"/>
     </row>
     <row r="7" spans="1:54" ht="18.75" customHeight="1">
       <c r="Z7" s="36"/>
+      <c r="AD7" s="36"/>
       <c r="AF7" s="14"/>
       <c r="AG7" s="49"/>
-      <c r="AH7" s="49"/>
+      <c r="AI7" s="36"/>
+      <c r="AJ7" s="36"/>
       <c r="AS7" s="36"/>
       <c r="AZ7" s="14"/>
       <c r="BB7" s="14"/>
     </row>
     <row r="8" spans="1:54" ht="18.75" customHeight="1">
       <c r="Z8" s="36"/>
+      <c r="AD8" s="36"/>
       <c r="AF8" s="14"/>
       <c r="AG8" s="14"/>
-      <c r="AH8" s="14"/>
+      <c r="AI8" s="36"/>
+      <c r="AJ8" s="36"/>
       <c r="AS8" s="36"/>
     </row>
     <row r="9" spans="1:54" ht="18.75" customHeight="1">
@@ -6432,6 +6457,61 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -6440,61 +6520,6 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>